<commit_message>
(NCIOCPL#124) Fixed data errors for citations and language toggle.
</commit_message>
<xml_diff>
--- a/test-data/citations-data.xlsx
+++ b/test-data/citations-data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB4F7AF-6C93-49A4-A32E-957E2D827E5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85462BB2-4359-42CE-9A5A-876799E7874D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="19185" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_citations" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>path</t>
   </si>
@@ -53,9 +53,6 @@
     <t>/espanol/noticias/comunicados-de-prensa/2018/leucemia-llc-ibrutinib-estudio</t>
   </si>
   <si>
-    <t>Referencias</t>
-  </si>
-  <si>
     <t>Selected References</t>
   </si>
   <si>
@@ -162,6 +159,12 @@
   </si>
   <si>
     <t>Video</t>
+  </si>
+  <si>
+    <t>Bibliografía selecta</t>
+  </si>
+  <si>
+    <t>Bibliografía</t>
   </si>
 </sst>
 </file>
@@ -501,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -541,10 +544,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,15 +561,15 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -575,10 +578,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,50 +589,50 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -645,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693BD2D3-6348-48F5-98A9-0A4DB7F6917A}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,10 +672,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -680,10 +683,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -691,10 +694,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -702,10 +705,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -713,10 +716,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -724,10 +727,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -735,10 +738,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -746,10 +749,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -757,10 +760,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -768,10 +771,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -779,10 +782,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -790,10 +793,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -801,10 +804,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -812,10 +815,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -823,10 +826,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -834,10 +837,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -845,10 +848,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
         <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>

</xml_diff>